<commit_message>
New Features Code of Vendor Tab
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/vib/testdata/KiranTestData.xlsx
+++ b/src/main/java/com/qa/vib/testdata/KiranTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -290,15 +290,6 @@
     <t>AML Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Per Customer Transaction  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Per City Customer Transaction </t>
-  </si>
-  <si>
-    <t>Per State Customer Transaction</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -404,6 +395,15 @@
   </si>
   <si>
     <t>ASCII characters as well as the space character</t>
+  </si>
+  <si>
+    <t>Per Customer Transaction in Town</t>
+  </si>
+  <si>
+    <t>Per Customer Transaction in City</t>
+  </si>
+  <si>
+    <t>Per Customer Transaction in MetroCity</t>
   </si>
 </sst>
 </file>
@@ -990,12 +990,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1022,16 +1022,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,60 +1277,60 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:4" ht="79.5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B4" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>118</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>121</v>
       </c>
       <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
@@ -1344,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1358,26 +1358,26 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2101,14 +2101,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J2" sqref="A1:J4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="9" width="26.28515625" style="12" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" style="12" customWidth="1"/>
     <col min="11" max="14" width="11.42578125" style="11" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="11"/>
   </cols>
@@ -2147,34 +2147,34 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="J2" s="14" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2205,8 +2205,8 @@
       <c r="I3" s="3">
         <v>180000</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>88</v>
+      <c r="J3" s="14" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2237,8 +2237,8 @@
       <c r="I4" s="3">
         <v>1800000</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>89</v>
+      <c r="J4" s="14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2279,37 +2279,37 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>